<commit_message>
[US BD04] Atualização do código de importação dos dados.
</commit_message>
<xml_diff>
--- a/docs/bddad/us-bd04/legacy-data-scripts-v0.xlsx
+++ b/docs/bddad/us-bd04/legacy-data-scripts-v0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anaog\OneDrive\Ambiente de Trabalho\segundo ano\primeiro semestre\sem3pi2023_24_g073\docs\bddad\us-bd04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF5B4EC-D3FA-41C1-991F-729F6F6F51C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CF5A60-1559-493D-95BA-0B83DE26E1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{ACBD79A1-D35B-4D3E-A78E-4F35CA726952}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ACBD79A1-D35B-4D3E-A78E-4F35CA726952}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantas" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="243">
   <si>
     <t>Prunus domestica</t>
   </si>
@@ -755,6 +755,24 @@
   </si>
   <si>
     <t>TipoUnidade</t>
+  </si>
+  <si>
+    <t>table_ name</t>
+  </si>
+  <si>
+    <t>Classificacao</t>
+  </si>
+  <si>
+    <t>ConstituicaoQuimica</t>
+  </si>
+  <si>
+    <t>SistemaDeRega</t>
+  </si>
+  <si>
+    <t>TipoCultura</t>
+  </si>
+  <si>
+    <t>TipoOperacaoAgricola</t>
   </si>
 </sst>
 </file>
@@ -794,7 +812,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -837,6 +855,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -850,7 +898,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -870,6 +918,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1224,7 +1279,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA74F46-7FB7-481B-9DAE-CE325D568C4A}">
   <dimension ref="A1:Y189"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H127" sqref="H127"/>
     </sheetView>
   </sheetViews>
@@ -6035,10 +6090,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD8BE3C6-089F-4A17-B7E6-182E6A73873F}">
-  <dimension ref="A1:R48"/>
+  <dimension ref="A1:R69"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M67" sqref="M67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6584,6 +6639,21 @@
         <v>231</v>
       </c>
       <c r="D24" s="8"/>
+      <c r="H24" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="J24" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="str">
@@ -6593,6 +6663,18 @@
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
+      <c r="H25" s="18" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;J24&amp; "(classificacao) VALUES ('" &amp;D2&amp; "');"</f>
+        <v>INSERT INTO Classificacao(classificacao) VALUES ('Fitofármaco');</v>
+      </c>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="str">
@@ -6602,6 +6684,18 @@
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
+      <c r="H26" s="18" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;J24&amp; "(classificacao) VALUES ('" &amp;D4&amp; "');"</f>
+        <v>INSERT INTO Classificacao(classificacao) VALUES ('Adubo');</v>
+      </c>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="str">
@@ -6611,6 +6705,18 @@
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
+      <c r="H27" s="18" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;J24&amp; "(classificacao) VALUES ('" &amp;D8&amp; "');"</f>
+        <v>INSERT INTO Classificacao(classificacao) VALUES ('Corretor');</v>
+      </c>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="str">
@@ -6791,6 +6897,275 @@
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
       <c r="G48" s="10"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="13" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$C$51&amp; "(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('" &amp;F2&amp; "', 1, '%', " &amp;TEXT(SUBSTITUTE(G2, "%", "") * 1000, "0.0")&amp; ");"</f>
+        <v>INSERT INTO ConstituicaoQuimica(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('CU', 1, '%', 20.0);</v>
+      </c>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="13" t="str">
+        <f t="shared" ref="A53" si="1" xml:space="preserve"> "INSERT INTO " &amp;$C$51&amp; "(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('" &amp;F3&amp; "', 1, '%', " &amp;TEXT(SUBSTITUTE(G3, "%", "") * 1000, "0.0")&amp; ");"</f>
+        <v>INSERT INTO ConstituicaoQuimica(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('S', 1, '%', 80.0);</v>
+      </c>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="13" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$C$51&amp; "(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('" &amp;F4&amp; "', 1, '%', " &amp;TEXT(SUBSTITUTE(G4, "%", "") * 1000, "0.0")&amp; ");"</f>
+        <v>INSERT INTO ConstituicaoQuimica(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('K', 1, '%', 24.9);</v>
+      </c>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="13" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$C$51&amp; "(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('" &amp;H4&amp; "', 1, '%', " &amp;TEXT(SUBSTITUTE(I4, "%", "") * 1000, "0.0")&amp; ");"</f>
+        <v>INSERT INTO ConstituicaoQuimica(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('Mg', 1, '%', 6.0);</v>
+      </c>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="13" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$C$51&amp; "(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('" &amp;J4&amp; "', 1, '%', " &amp;TEXT(SUBSTITUTE(K4, "%", "") * 1000, "0.0")&amp; ");"</f>
+        <v>INSERT INTO ConstituicaoQuimica(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('S', 1, '%', 17.6);</v>
+      </c>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="13" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$C$51&amp; "(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('" &amp;F5&amp; "', 1, '%', " &amp;TEXT(SUBSTITUTE(G5, "%", "") * 1000, "0.0")&amp; ");"</f>
+        <v>INSERT INTO ConstituicaoQuimica(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('Mg', 1, '%', 15.1);</v>
+      </c>
+      <c r="B57" s="13"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="13" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$C$51&amp; "(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('" &amp;H5&amp; "', 1, '%', " &amp;TEXT(SUBSTITUTE(I5, "%", "") * 1000, "0.0")&amp; ");"</f>
+        <v>INSERT INTO ConstituicaoQuimica(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('S', 1, '%', 20.8);</v>
+      </c>
+      <c r="B58" s="13"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="13" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$C$51&amp; "(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('" &amp;F6&amp; "', 1, '%', " &amp;TEXT(SUBSTITUTE(G6, "%", "") * 1000, "0.0")&amp; ");"</f>
+        <v>INSERT INTO ConstituicaoQuimica(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('Mg', 1, '%', 9.0);</v>
+      </c>
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="13" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$C$51&amp; "(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('" &amp;H6&amp; "', 1, '%', " &amp;TEXT(SUBSTITUTE(I6, "%", "") * 1000, "0.0")&amp; ");"</f>
+        <v>INSERT INTO ConstituicaoQuimica(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('S', 1, '%', 12.4);</v>
+      </c>
+      <c r="B60" s="13"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="13" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$C$51&amp; "(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('" &amp;J6&amp; "', 1, '%', " &amp;TEXT(SUBSTITUTE(K6, "%", "") * 1000, "0.0")&amp; ");"</f>
+        <v>INSERT INTO ConstituicaoQuimica(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('B', 1, '%', 0.9);</v>
+      </c>
+      <c r="B61" s="13"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="13" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$C$51&amp; "(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('" &amp;L6&amp; "', 1, '%', " &amp;TEXT(SUBSTITUTE(M6, "%", "") * 1000, "0.0")&amp; ");"</f>
+        <v>INSERT INTO ConstituicaoQuimica(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('Mn', 1, '%', 1.0);</v>
+      </c>
+      <c r="B62" s="13"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="13"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="13" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$C$51&amp; "(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('" &amp;F7&amp; "', 1, '%', " &amp;TEXT(SUBSTITUTE(G7, "%", "") * 1000, "0.0")&amp; ");"</f>
+        <v>INSERT INTO ConstituicaoQuimica(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('Mg', 1, '%', 9.6);</v>
+      </c>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="13" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$C$51&amp; "(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('" &amp;H7&amp; "', 1, '%', " &amp;TEXT(SUBSTITUTE(I7, "%", "") * 1000, "0.0")&amp; ");"</f>
+        <v>INSERT INTO ConstituicaoQuimica(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('S', 1, '%', 13.0);</v>
+      </c>
+      <c r="B64" s="13"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="13"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="13" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$C$51&amp; "(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('" &amp;F8&amp; "', 1, '%', " &amp;TEXT(SUBSTITUTE(G8, "%", "") * 1000, "0.0")&amp; ");"</f>
+        <v>INSERT INTO ConstituicaoQuimica(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('CaCO3', 1, '%', 88.2);</v>
+      </c>
+      <c r="B65" s="13"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="13" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$C$51&amp; "(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('" &amp;H8&amp; "', 1, '%', " &amp;TEXT(SUBSTITUTE(I8, "%", "") * 1000, "0.0")&amp; ");"</f>
+        <v>INSERT INTO ConstituicaoQuimica(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('MgCO3', 1, '%', 1.9);</v>
+      </c>
+      <c r="B66" s="13"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="13"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" s="13" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$C$51&amp; "(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('" &amp;F9&amp; "', 1, '%', " &amp;TEXT(SUBSTITUTE(G9, "%", "") * 1000, "0.0")&amp; ");"</f>
+        <v>INSERT INTO ConstituicaoQuimica(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('CaCO3', 1, '%', 71.7);</v>
+      </c>
+      <c r="B67" s="13"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="13" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$C$51&amp; "(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('" &amp;H9&amp; "', 1, '%', " &amp;TEXT(SUBSTITUTE(I9, "%", "") * 1000, "0.0")&amp; ");"</f>
+        <v>INSERT INTO ConstituicaoQuimica(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('MgCO3', 1, '%', 14.8);</v>
+      </c>
+      <c r="B68" s="13"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" s="13" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$C$51&amp; "(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('" &amp;J9&amp; "', 1, '%', " &amp;TEXT(SUBSTITUTE(K9, "%", "") * 1000, "0.0")&amp; ");"</f>
+        <v>INSERT INTO ConstituicaoQuimica(formulaQuimica, idFichaTecnica, designacaoUnidade, quantidade) VALUES ('MgO', 1, '%', 7.9);</v>
+      </c>
+      <c r="B69" s="13"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6800,10 +7175,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B01B56-4BBE-4836-8DCB-B3AF8DABE0BB}">
-  <dimension ref="A1:V22"/>
+  <dimension ref="A1:V28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7244,6 +7619,39 @@
       <c r="O22" s="10"/>
       <c r="P22" s="10"/>
     </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K26" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="L26" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="M26" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K27" s="10" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$M$26&amp; "(idEdificio) VALUES (" &amp;A12&amp; ");"</f>
+        <v>INSERT INTO SistemaDeRega(idEdificio) VALUES (301);</v>
+      </c>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7253,10 +7661,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{246DE277-EC3F-46EA-8D39-A978B7AEA5AE}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7584,43 +7992,276 @@
         <v>INSERT INTO Cultura(idCultura, variedade, nomeComum, idParcela) values(1011, Campo da bouça, Tremoço Amarelo, 101);</v>
       </c>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B15" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B16" s="10" t="str">
+        <f>"INSERT INTO " &amp;$C$15&amp; "('" &amp;E2&amp; "');"</f>
+        <v>INSERT INTO table_name('42649');</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B17" s="10" t="str">
+        <f>"INSERT INTO " &amp;$C$15&amp; "('" &amp;E8&amp; "');"</f>
+        <v>INSERT INTO table_name('44114');</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="13" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$C$21&amp; "(idParcela, idCultura, designacaoUnidade, dataInicial, dataFinal, quantidade) VALUES (" &amp;A2&amp;", 3, '" &amp;H2&amp; "', TO_DATE('"&amp;TEXT(E2,"DD/MM/AAAA")&amp;"', 'DD/MM/YYYY'), "&amp;IF(ISBLANK(F2),"null","TO_DATE('"&amp;TEXT(F2,"DD/MM/AAAA")&amp;"', 'DD/MM/YYYY')")&amp; ", " &amp;G2&amp; ");"</f>
+        <v>INSERT INTO CulturaInstalada(idParcela, idCultura, designacaoUnidade, dataInicial, dataFinal, quantidade) VALUES (102, 3, 'un', TO_DATE('06/10/2016', 'DD/MM/YYYY'), null, 30);</v>
+      </c>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="13" t="str">
+        <f t="shared" ref="A23:A31" si="1" xml:space="preserve"> "INSERT INTO " &amp;$C$21&amp; "(idParcela, idCultura, designacaoUnidade, dataInicial, dataFinal, quantidade) VALUES (" &amp;A3&amp;", 3, '" &amp;H3&amp; "', TO_DATE('"&amp;TEXT(E3,"DD/MM/AAAA")&amp;"', 'DD/MM/YYYY'), "&amp;IF(ISBLANK(F3),"null","TO_DATE('"&amp;TEXT(F3,"DD/MM/AAAA")&amp;"', 'DD/MM/YYYY')")&amp; ", " &amp;G3&amp; ");"</f>
+        <v>INSERT INTO CulturaInstalada(idParcela, idCultura, designacaoUnidade, dataInicial, dataFinal, quantidade) VALUES (102, 3, 'un', TO_DATE('10/10/2016', 'DD/MM/YYYY'), null, 20);</v>
+      </c>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO CulturaInstalada(idParcela, idCultura, designacaoUnidade, dataInicial, dataFinal, quantidade) VALUES (104, 3, 'un', TO_DATE('07/01/2017', 'DD/MM/YYYY'), null, 90);</v>
+      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO CulturaInstalada(idParcela, idCultura, designacaoUnidade, dataInicial, dataFinal, quantidade) VALUES (104, 3, 'un', TO_DATE('08/01/2017', 'DD/MM/YYYY'), null, 60);</v>
+      </c>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO CulturaInstalada(idParcela, idCultura, designacaoUnidade, dataInicial, dataFinal, quantidade) VALUES (104, 3, 'un', TO_DATE('08/01/2017', 'DD/MM/YYYY'), null, 40);</v>
+      </c>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO CulturaInstalada(idParcela, idCultura, designacaoUnidade, dataInicial, dataFinal, quantidade) VALUES (104, 3, 'un', TO_DATE('10/12/2018', 'DD/MM/YYYY'), null, 30);</v>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO CulturaInstalada(idParcela, idCultura, designacaoUnidade, dataInicial, dataFinal, quantidade) VALUES (101, 3, 'ha', TO_DATE('10/10/2020', 'DD/MM/YYYY'), TO_DATE('30/03/2021', 'DD/MM/YYYY'), 1,1);</v>
+      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO CulturaInstalada(idParcela, idCultura, designacaoUnidade, dataInicial, dataFinal, quantidade) VALUES (101, 3, 'ha', TO_DATE('10/04/2021', 'DD/MM/YYYY'), TO_DATE('12/08/2021', 'DD/MM/YYYY'), 0,9);</v>
+      </c>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO CulturaInstalada(idParcela, idCultura, designacaoUnidade, dataInicial, dataFinal, quantidade) VALUES (101, 3, 'ha', TO_DATE('15/04/2021', 'DD/MM/YYYY'), TO_DATE('21/08/2021', 'DD/MM/YYYY'), 0,9);</v>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="13" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO CulturaInstalada(idParcela, idCultura, designacaoUnidade, dataInicial, dataFinal, quantidade) VALUES (101, 3, 'ha', TO_DATE('03/10/2021', 'DD/MM/YYYY'), TO_DATE('05/04/2022', 'DD/MM/YYYY'), 1,1);</v>
+      </c>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H11">
@@ -7634,10 +8275,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8273E431-88A0-4D26-AA21-9E0D94FE2923}">
-  <dimension ref="A1:M82"/>
+  <dimension ref="A1:T82"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="N48" sqref="N48"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8014,7 +8655,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>101</v>
       </c>
@@ -8037,7 +8678,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>104</v>
       </c>
@@ -8060,7 +8701,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>104</v>
       </c>
@@ -8083,7 +8724,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>104</v>
       </c>
@@ -8105,8 +8746,23 @@
       <c r="H20" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L20" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="M20" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="N20" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="22"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="22"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>104</v>
       </c>
@@ -8128,8 +8784,20 @@
       <c r="H21" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L21" s="23" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$N$20&amp;  "(designacaoOperacaoAgricola) VALUES ('" &amp;C2&amp; "');"</f>
+        <v>INSERT INTO TipoOperacaoAgricola(designacaoOperacaoAgricola) VALUES ('Plantação');</v>
+      </c>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23"/>
+      <c r="S21" s="23"/>
+      <c r="T21" s="23"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>101</v>
       </c>
@@ -8145,8 +8813,20 @@
       <c r="F22" s="1">
         <v>44472</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L22" s="23" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$N$20&amp;  "(designacaoOperacaoAgricola) VALUES ('" &amp;C9&amp; "');"</f>
+        <v>INSERT INTO TipoOperacaoAgricola(designacaoOperacaoAgricola) VALUES ('Poda');</v>
+      </c>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="23"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>104</v>
       </c>
@@ -8168,8 +8848,20 @@
       <c r="H23" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L23" s="23" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$N$20&amp;  "(designacaoOperacaoAgricola) VALUES ('" &amp;C9&amp; "');"</f>
+        <v>INSERT INTO TipoOperacaoAgricola(designacaoOperacaoAgricola) VALUES ('Poda');</v>
+      </c>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="23"/>
+      <c r="T23" s="23"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>104</v>
       </c>
@@ -8191,8 +8883,20 @@
       <c r="H24" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L24" s="23" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$N$20&amp;  "(designacaoOperacaoAgricola) VALUES ('" &amp;C13&amp; "');"</f>
+        <v>INSERT INTO TipoOperacaoAgricola(designacaoOperacaoAgricola) VALUES ('Incorporação no solo');</v>
+      </c>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>104</v>
       </c>
@@ -8214,8 +8918,20 @@
       <c r="H25" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L25" s="23" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$N$20&amp;  "(designacaoOperacaoAgricola) VALUES ('" &amp;C15&amp; "');"</f>
+        <v>INSERT INTO TipoOperacaoAgricola(designacaoOperacaoAgricola) VALUES ('Fertilização');</v>
+      </c>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="23"/>
+      <c r="S25" s="23"/>
+      <c r="T25" s="23"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>104</v>
       </c>
@@ -8237,8 +8953,20 @@
       <c r="H26" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L26" s="23" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$N$20&amp;  "(designacaoOperacaoAgricola) VALUES ('" &amp;C16&amp; "');"</f>
+        <v>INSERT INTO TipoOperacaoAgricola(designacaoOperacaoAgricola) VALUES ('Rega');</v>
+      </c>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="23"/>
+      <c r="R26" s="23"/>
+      <c r="S26" s="23"/>
+      <c r="T26" s="23"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>104</v>
       </c>
@@ -8260,8 +8988,20 @@
       <c r="H27" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="L27" s="23" t="str">
+        <f xml:space="preserve"> "INSERT INTO " &amp;$N$20&amp;  "(designacaoOperacaoAgricola) VALUES ('" &amp;C17&amp; "');"</f>
+        <v>INSERT INTO TipoOperacaoAgricola(designacaoOperacaoAgricola) VALUES ('Colheita');</v>
+      </c>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="23"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="23"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>101</v>
       </c>
@@ -8278,7 +9018,7 @@
         <v>44656</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>101</v>
       </c>
@@ -8295,7 +9035,7 @@
         <v>44661</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>104</v>
       </c>
@@ -8324,7 +9064,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>101</v>
       </c>
@@ -8347,7 +9087,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>104</v>
       </c>
@@ -9461,14 +10201,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="8baafd8b-20f3-4709-bc83-186ae70c422f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001FE1D12FE0EBDA4CB61620080A85CBAE" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="29a33cb73e06d038149e1c9d44f381e8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c9101efd-7fb7-4b65-82fa-5268cef970aa" xmlns:ns4="8baafd8b-20f3-4709-bc83-186ae70c422f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="959936be2cfdc50d0a8ac64b81b8b25a" ns3:_="" ns4:_="">
     <xsd:import namespace="c9101efd-7fb7-4b65-82fa-5268cef970aa"/>
@@ -9651,6 +10383,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="8baafd8b-20f3-4709-bc83-186ae70c422f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -9661,23 +10401,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA37870F-1997-46E6-ABF3-D972D5619E05}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="8baafd8b-20f3-4709-bc83-186ae70c422f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c9101efd-7fb7-4b65-82fa-5268cef970aa"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{123E14B8-9922-4582-B143-574A2CB640AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9696,6 +10419,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA37870F-1997-46E6-ABF3-D972D5619E05}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="8baafd8b-20f3-4709-bc83-186ae70c422f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c9101efd-7fb7-4b65-82fa-5268cef970aa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E8E74F1-259B-4A8D-986B-B2E55FA52FD9}">
   <ds:schemaRefs>

</xml_diff>